<commit_message>
Fixed read, write and apply_limitations bug
</commit_message>
<xml_diff>
--- a/specsMalawi.xlsx
+++ b/specsMalawi.xlsx
@@ -611,8 +611,11 @@
       <c r="F2">
         <v>0.16</v>
       </c>
+      <c r="G2">
+        <v>3332.460923935724</v>
+      </c>
       <c r="H2">
-        <v>0.05</v>
+        <v>0.1598809861329305</v>
       </c>
       <c r="I2">
         <v>26578247</v>
@@ -654,19 +657,19 @@
         <v>0.09</v>
       </c>
       <c r="V2">
-        <v>5000</v>
+        <v>0.7123034778733883</v>
       </c>
       <c r="W2">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="X2">
         <v>1</v>
       </c>
       <c r="Y2">
-        <v>1.99402290566502</v>
+        <v>5</v>
       </c>
       <c r="Z2">
-        <v>0.08484773030071693</v>
+        <v>0.5</v>
       </c>
       <c r="AA2">
         <v>10000</v>

</xml_diff>

<commit_message>
Move gridcapacitygenerationlimit to specs
</commit_message>
<xml_diff>
--- a/specsMalawi.xlsx
+++ b/specsMalawi.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>StartYear</t>
   </si>
@@ -122,13 +122,16 @@
   </si>
   <si>
     <t>Malawi</t>
+  </si>
+  <si>
+    <t>NewGridGenerationCapacityTimestepLimit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -176,13 +179,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -191,11 +208,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -269,6 +291,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -303,6 +326,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -478,14 +502,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AJ1" sqref="AJ1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -591,8 +617,11 @@
       <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="AJ1" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -612,7 +641,7 @@
         <v>0.16</v>
       </c>
       <c r="G2">
-        <v>3332.460923935724</v>
+        <v>3332.4609239357242</v>
       </c>
       <c r="H2">
         <v>0.1598809861329305</v>
@@ -657,7 +686,7 @@
         <v>0.09</v>
       </c>
       <c r="V2">
-        <v>0.7123034778733883</v>
+        <v>0.71230347787338832</v>
       </c>
       <c r="W2">
         <v>60</v>
@@ -679,6 +708,9 @@
       </c>
       <c r="AD2">
         <v>2600</v>
+      </c>
+      <c r="AJ2">
+        <v>9999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New grid distribution network calc
</commit_message>
<xml_diff>
--- a/specsMalawi.xlsx
+++ b/specsMalawi.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -118,20 +118,20 @@
     <t>Cap_Cost_SA_DS</t>
   </si>
   <si>
+    <t>NewGridGenerationCapacityTimestepLimit</t>
+  </si>
+  <si>
     <t>Country</t>
   </si>
   <si>
     <t>Malawi</t>
-  </si>
-  <si>
-    <t>NewGridGenerationCapacityTimestepLimit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -179,27 +179,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -208,16 +194,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -291,7 +272,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -326,7 +306,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -502,18 +481,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AJ1" sqref="AJ1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -617,13 +594,13 @@
       <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36">
+      <c r="A2" s="1" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="B2">
         <v>2015</v>
@@ -641,10 +618,10 @@
         <v>0.16</v>
       </c>
       <c r="G2">
-        <v>3332.4609239357242</v>
+        <v>1389.601701909612</v>
       </c>
       <c r="H2">
-        <v>0.1598809861329305</v>
+        <v>0.1599888484040377</v>
       </c>
       <c r="I2">
         <v>26578247</v>
@@ -686,10 +663,10 @@
         <v>0.09</v>
       </c>
       <c r="V2">
-        <v>0.71230347787338832</v>
+        <v>0.0986176933596884</v>
       </c>
       <c r="W2">
-        <v>60</v>
+        <v>44.22420440792517</v>
       </c>
       <c r="X2">
         <v>1</v>
@@ -701,10 +678,10 @@
         <v>0.5</v>
       </c>
       <c r="AA2">
-        <v>10000</v>
+        <v>4000</v>
       </c>
       <c r="AB2">
-        <v>2</v>
+        <v>4500</v>
       </c>
       <c r="AD2">
         <v>2600</v>

</xml_diff>

<commit_message>
Updated csv and specs file
</commit_message>
<xml_diff>
--- a/specsMalawi.xlsx
+++ b/specsMalawi.xlsx
@@ -618,10 +618,10 @@
         <v>0.16</v>
       </c>
       <c r="G2">
-        <v>1389.601701909612</v>
+        <v>1201.638031908821</v>
       </c>
       <c r="H2">
-        <v>0.1599888484040377</v>
+        <v>0.1599326748571309</v>
       </c>
       <c r="I2">
         <v>26578247</v>
@@ -663,7 +663,7 @@
         <v>0.09</v>
       </c>
       <c r="V2">
-        <v>0.0986176933596884</v>
+        <v>0.08998189082754326</v>
       </c>
       <c r="W2">
         <v>44.22420440792517</v>

</xml_diff>

<commit_message>
Bug fix start year
</commit_message>
<xml_diff>
--- a/specsMalawi.xlsx
+++ b/specsMalawi.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -130,8 +130,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,11 +194,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -272,6 +277,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -306,6 +312,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -481,14 +488,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -598,12 +607,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B2">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="C2">
         <v>2030</v>
@@ -618,10 +627,10 @@
         <v>0.16</v>
       </c>
       <c r="G2">
-        <v>1201.638031908834</v>
+        <v>1201.6380319088339</v>
       </c>
       <c r="H2">
-        <v>0.1599326748571324</v>
+        <v>0.15993267485713239</v>
       </c>
       <c r="I2">
         <v>26578247</v>
@@ -663,10 +672,10 @@
         <v>0.09</v>
       </c>
       <c r="V2">
-        <v>0.09879284494363139</v>
+        <v>9.8792844943631386E-2</v>
       </c>
       <c r="W2">
-        <v>32.83246120861349</v>
+        <v>32.832461208613488</v>
       </c>
       <c r="X2">
         <v>1</v>

</xml_diff>

<commit_message>
Made compatible with master branch
</commit_message>
<xml_diff>
--- a/specsMalawi.xlsx
+++ b/specsMalawi.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -130,8 +130,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,11 +194,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -272,6 +277,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -306,6 +312,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -481,14 +488,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -598,12 +607,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B2">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="C2">
         <v>2030</v>
@@ -618,10 +627,10 @@
         <v>0.16</v>
       </c>
       <c r="G2">
-        <v>1201.638031908821</v>
+        <v>1201.6380319088209</v>
       </c>
       <c r="H2">
-        <v>0.1599326748571309</v>
+        <v>0.15993267485713089</v>
       </c>
       <c r="I2">
         <v>26578247</v>
@@ -663,10 +672,10 @@
         <v>0.09</v>
       </c>
       <c r="V2">
-        <v>0.08998189082754326</v>
+        <v>8.9981890827543265E-2</v>
       </c>
       <c r="W2">
-        <v>44.22420440792517</v>
+        <v>44.224204407925171</v>
       </c>
       <c r="X2">
         <v>1</v>

</xml_diff>

<commit_message>
Reading demand from csv columns and elec calib modifications
</commit_message>
<xml_diff>
--- a/specsMalawi.xlsx
+++ b/specsMalawi.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -130,8 +130,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,16 +194,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -277,7 +272,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -312,7 +306,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -488,16 +481,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -607,7 +598,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -627,10 +618,10 @@
         <v>0.16</v>
       </c>
       <c r="G2">
-        <v>1201.6380319088209</v>
+        <v>2858.003227632393</v>
       </c>
       <c r="H2">
-        <v>0.15993267485713089</v>
+        <v>0.1598539884266991</v>
       </c>
       <c r="I2">
         <v>26578247</v>
@@ -672,25 +663,25 @@
         <v>0.09</v>
       </c>
       <c r="V2">
-        <v>8.9981890827543265E-2</v>
+        <v>0.09908597401481424</v>
       </c>
       <c r="W2">
-        <v>44.224204407925171</v>
+        <v>10</v>
       </c>
       <c r="X2">
         <v>1</v>
       </c>
       <c r="Y2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Z2">
         <v>0.5</v>
       </c>
       <c r="AA2">
-        <v>4000</v>
+        <v>6140.790349047872</v>
       </c>
       <c r="AB2">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="AD2">
         <v>2600</v>

</xml_diff>

<commit_message>
New method to calibrate electrified
</commit_message>
<xml_diff>
--- a/specsMalawi.xlsx
+++ b/specsMalawi.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>StartYear</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>NewGridGenerationCapacityTimestepLimit</t>
+  </si>
+  <si>
+    <t>Rural_elec_ratio</t>
+  </si>
+  <si>
+    <t>Urban_elec_ratio</t>
+  </si>
+  <si>
+    <t>rural_elec_ratio</t>
+  </si>
+  <si>
+    <t>urban_elec_ratio</t>
   </si>
   <si>
     <t>Country</t>
@@ -482,15 +494,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AN2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:40">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -597,10 +609,22 @@
       <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:40">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>2018</v>
@@ -663,7 +687,7 @@
         <v>0.09</v>
       </c>
       <c r="V2">
-        <v>0.09908597401481424</v>
+        <v>0.2067083252821392</v>
       </c>
       <c r="W2">
         <v>10</v>
@@ -688,6 +712,18 @@
       </c>
       <c r="AJ2">
         <v>9999999</v>
+      </c>
+      <c r="AK2">
+        <v>0.039</v>
+      </c>
+      <c r="AL2">
+        <v>0.487</v>
+      </c>
+      <c r="AM2">
+        <v>2.139405086654099</v>
+      </c>
+      <c r="AN2">
+        <v>1.754799943289467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ability to incorporate urban centers and clusters
</commit_message>
<xml_diff>
--- a/specsMalawi.xlsx
+++ b/specsMalawi.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -142,8 +142,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,11 +206,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -284,6 +289,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -318,6 +324,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -493,14 +500,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AN7" sqref="AN7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -622,7 +631,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -642,7 +651,7 @@
         <v>0.16</v>
       </c>
       <c r="G2">
-        <v>2858.003227632393</v>
+        <v>2858.0032276323932</v>
       </c>
       <c r="H2">
         <v>0.1598539884266991</v>
@@ -714,16 +723,16 @@
         <v>9999999</v>
       </c>
       <c r="AK2">
-        <v>0.039</v>
+        <v>3.9E-2</v>
       </c>
       <c r="AL2">
-        <v>0.487</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="AM2">
-        <v>2.139405086654099</v>
+        <v>0.46741966083849035</v>
       </c>
       <c r="AN2">
-        <v>1.754799943289467</v>
+        <v>0.56986553015578867</v>
       </c>
     </row>
   </sheetData>

</xml_diff>